<commit_message>
Worked On Insert statements
</commit_message>
<xml_diff>
--- a/DataBaseRecords.xlsx
+++ b/DataBaseRecords.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SEN381_Project\PremierService-Solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matin Personal StudyProjects\PremierService-Solutions-FrontEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EEE00B-5813-40D9-9246-9F249C040281}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D4D635-9845-4C7E-B020-EDF09BC68E6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1005" windowWidth="28800" windowHeight="15435" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Address" sheetId="1" r:id="rId1"/>
@@ -66,26 +66,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="192">
   <si>
     <t>streetName</t>
   </si>
   <si>
-    <t>Foxhound</t>
-  </si>
-  <si>
-    <t>Maple</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>Maxwell</t>
-  </si>
-  <si>
-    <t>Church</t>
-  </si>
-  <si>
     <t>Midrand</t>
   </si>
   <si>
@@ -101,15 +86,6 @@
     <t>Brooklyn</t>
   </si>
   <si>
-    <t>Gauteng</t>
-  </si>
-  <si>
-    <t>Western Cape</t>
-  </si>
-  <si>
-    <t>Eastern Cape</t>
-  </si>
-  <si>
     <t>contactNumber</t>
   </si>
   <si>
@@ -170,15 +146,9 @@
     <t>2000-12-01</t>
   </si>
   <si>
-    <t>1990-02-19</t>
-  </si>
-  <si>
     <t>1980-06-02</t>
   </si>
   <si>
-    <t>1999-10-22</t>
-  </si>
-  <si>
     <t>2002-02-20</t>
   </si>
   <si>
@@ -636,6 +606,42 @@
   </si>
   <si>
     <t>contractType</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>johannesburg</t>
+  </si>
+  <si>
+    <t>Pretoria</t>
+  </si>
+  <si>
+    <t>capetown</t>
+  </si>
+  <si>
+    <t>1990-02-01</t>
+  </si>
+  <si>
+    <t>1999-10-02</t>
+  </si>
+  <si>
+    <t>2002-02-03</t>
+  </si>
+  <si>
+    <t>21 Foxhound</t>
+  </si>
+  <si>
+    <t>32 Maple</t>
+  </si>
+  <si>
+    <t>63 Main</t>
+  </si>
+  <si>
+    <t>92 Maxwell</t>
+  </si>
+  <si>
+    <t>55 Church</t>
   </si>
 </sst>
 </file>
@@ -680,11 +686,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -966,99 +973,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="132" style="4" customWidth="1"/>
+    <col min="7" max="16" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>181</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>1684</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
       <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>1932</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>183</v>
       </c>
       <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
         <v>1029</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>7102</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
         <v>1984</v>
       </c>
     </row>
@@ -1079,22 +1107,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F1" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1207,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A729D5E5-EBA3-4AD4-89B3-6D680D0AD05C}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1215,22 +1243,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1240,200 +1268,200 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285A87D0-6993-4E9A-92DB-3C38401DBA37}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="C1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A4" sqref="A4:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
+    <row r="1" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3">
+        <v>9861237651092</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1348302832952</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3">
+        <v>8305283029467</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="3">
+        <v>7502837592035</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="3">
-        <v>9861237651092</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1348302832952</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="H6" s="3">
+        <v>9305832739295</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
         <v>30</v>
-      </c>
-      <c r="F4" s="3">
-        <v>8305283029467</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="3">
-        <v>7502837592035</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="3">
-        <v>9305832739295</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{823BB252-E784-4809-9491-8163236AC9CE}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{91822FBF-8BBC-46E8-AD23-268479C18DF2}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{31AD3656-8BD8-4E53-93F3-4E6D9B0F3726}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{9C713FE9-3584-44D3-A948-B3D59640D65B}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{17631E80-A551-4CF4-B424-0AE6775C57A1}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{823BB252-E784-4809-9491-8163236AC9CE}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{91822FBF-8BBC-46E8-AD23-268479C18DF2}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{31AD3656-8BD8-4E53-93F3-4E6D9B0F3726}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{9C713FE9-3584-44D3-A948-B3D59640D65B}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{17631E80-A551-4CF4-B424-0AE6775C57A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1444,57 +1472,62 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="117.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1521,51 +1554,51 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="H1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1573,25 +1606,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1599,25 +1632,25 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1625,25 +1658,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1651,25 +1684,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1677,7 +1710,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1707,39 +1740,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1747,19 +1780,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1767,19 +1800,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1787,19 +1820,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1807,19 +1840,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1842,27 +1875,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1878,7 +1911,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1894,7 +1927,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1910,7 +1943,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1926,7 +1959,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1935,10 +1968,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F6">
         <v>20000</v>
@@ -1961,50 +1994,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2024,107 +2057,107 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F4" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" t="s">
         <v>146</v>
       </c>
-      <c r="D5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" t="s">
-        <v>156</v>
-      </c>
       <c r="F5" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" t="s">
         <v>147</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>151</v>
-      </c>
-      <c r="E6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2144,16 +2177,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2168,7 +2201,7 @@
         <v>Broken pipes</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2216,7 @@
         <v>Garden needs weeds removed</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2198,7 +2231,7 @@
         <v>Light switch won't work</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2213,7 +2246,7 @@
         <v>Printer jammed</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2228,7 +2261,7 @@
         <v>Wall has paint chips</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>